<commit_message>
Update biz plan, biz model
</commit_message>
<xml_diff>
--- a/Documents/Roles.xlsx
+++ b/Documents/Roles.xlsx
@@ -1,26 +1,112 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>This document indicates the roles of each member in the team. The role can be changed afterwards to fit with the condition of the company</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>Geographic roles</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>Functional roles include:</t>
+  </si>
+  <si>
+    <t>Area manager</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Negotiation</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>Logistics</t>
+  </si>
+  <si>
+    <t>R&amp;D</t>
+  </si>
+  <si>
+    <t>Etc.</t>
+  </si>
+  <si>
+    <t>Home Office (Leich.)</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -43,13 +129,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -343,37 +437,147 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="28.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:E2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>